<commit_message>
add TruthfulQA L11 result to final excel
</commit_message>
<xml_diff>
--- a/Final Evaluation/merged_averages.xlsx
+++ b/Final Evaluation/merged_averages.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/honganhnguyen/Documents/Study/Intelligent Systems/COS30018-Mitigate-Hallucination/Final Evaluation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pink\Documents\Study\Intelligent Systems\COS30018-Mitigate-Hallucination\Final Evaluation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59CD34D6-C042-8548-A71C-7EC5BA1630CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4D1DDC9-286A-474E-A12E-9FD9B117C72A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" activeTab="1" xr2:uid="{6A54DB1A-C799-4116-88B3-55941F091460}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21840" activeTab="2" xr2:uid="{6A54DB1A-C799-4116-88B3-55941F091460}"/>
   </bookViews>
   <sheets>
     <sheet name="Med-Halt" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="74">
   <si>
     <t>FAKE Accuracy_pred</t>
   </si>
@@ -253,6 +253,9 @@
   </si>
   <si>
     <t>Average</t>
+  </si>
+  <si>
+    <t>L11</t>
   </si>
 </sst>
 </file>
@@ -736,9 +739,10 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -861,8 +865,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{E80E8143-C169-4C06-AC7B-944234CB091B}" name="Table3" displayName="Table3" ref="A1:E21" totalsRowShown="0">
-  <autoFilter ref="A1:E21" xr:uid="{E80E8143-C169-4C06-AC7B-944234CB091B}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{E80E8143-C169-4C06-AC7B-944234CB091B}" name="Table3" displayName="Table3" ref="A1:E22" totalsRowShown="0">
+  <autoFilter ref="A1:E22" xr:uid="{E80E8143-C169-4C06-AC7B-944234CB091B}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{19784234-74A6-4125-AAB2-A9F90523DD18}" name="model"/>
     <tableColumn id="2" xr3:uid="{43A76758-9B3A-4B48-B95E-240B62A5A2C2}" name="bleu_acc"/>
@@ -1202,30 +1206,30 @@
       <selection pane="bottomRight" activeCell="R19" sqref="R19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19" customWidth="1"/>
     <col min="2" max="2" width="21" customWidth="1"/>
-    <col min="3" max="3" width="19.5" customWidth="1"/>
-    <col min="4" max="4" width="17.83203125" customWidth="1"/>
-    <col min="5" max="5" width="20.5" customWidth="1"/>
+    <col min="3" max="3" width="19.42578125" customWidth="1"/>
+    <col min="4" max="4" width="17.85546875" customWidth="1"/>
+    <col min="5" max="5" width="20.42578125" customWidth="1"/>
     <col min="6" max="6" width="15" customWidth="1"/>
-    <col min="7" max="7" width="14.5" customWidth="1"/>
+    <col min="7" max="7" width="14.42578125" customWidth="1"/>
     <col min="8" max="8" width="20" customWidth="1"/>
-    <col min="9" max="9" width="18.5" customWidth="1"/>
-    <col min="10" max="10" width="16.83203125" customWidth="1"/>
-    <col min="11" max="11" width="19.5" customWidth="1"/>
+    <col min="9" max="9" width="18.42578125" customWidth="1"/>
+    <col min="10" max="10" width="16.85546875" customWidth="1"/>
+    <col min="11" max="11" width="19.42578125" customWidth="1"/>
     <col min="12" max="12" width="14" customWidth="1"/>
-    <col min="13" max="13" width="13.5" customWidth="1"/>
-    <col min="14" max="14" width="21.5" customWidth="1"/>
+    <col min="13" max="13" width="13.42578125" customWidth="1"/>
+    <col min="14" max="14" width="21.42578125" customWidth="1"/>
     <col min="15" max="15" width="20" customWidth="1"/>
-    <col min="16" max="16" width="18.5" customWidth="1"/>
+    <col min="16" max="16" width="18.42578125" customWidth="1"/>
     <col min="17" max="17" width="21" customWidth="1"/>
-    <col min="18" max="18" width="15.5" customWidth="1"/>
-    <col min="19" max="19" width="15.1640625" customWidth="1"/>
+    <col min="18" max="18" width="15.42578125" customWidth="1"/>
+    <col min="19" max="19" width="15.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>24</v>
       </c>
@@ -1287,7 +1291,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>38</v>
       </c>
@@ -1350,7 +1354,7 @@
         <v>0.37580490333333327</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>39</v>
       </c>
@@ -1413,7 +1417,7 @@
         <v>0.10723553711111113</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>28</v>
       </c>
@@ -1476,7 +1480,7 @@
         <v>0.22008164250000004</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>29</v>
       </c>
@@ -1539,7 +1543,7 @@
         <v>0.26972544950000005</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>30</v>
       </c>
@@ -1602,7 +1606,7 @@
         <v>0.12725569372222223</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>31</v>
       </c>
@@ -1665,7 +1669,7 @@
         <v>0.10757410033333331</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>32</v>
       </c>
@@ -1728,7 +1732,7 @@
         <v>0.11830283011111112</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>33</v>
       </c>
@@ -1791,7 +1795,7 @@
         <v>0.37580490333333327</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>34</v>
       </c>
@@ -1854,7 +1858,7 @@
         <v>0.41647101922222235</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>35</v>
       </c>
@@ -1917,7 +1921,7 @@
         <v>0.40624996605555552</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>36</v>
       </c>
@@ -1980,7 +1984,7 @@
         <v>0.34464008411111113</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>37</v>
       </c>
@@ -2055,21 +2059,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D06B564-6277-499B-8EA6-CD4A445B41D3}">
   <dimension ref="A1:H22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="16.1640625" customWidth="1"/>
-    <col min="3" max="3" width="14.5" customWidth="1"/>
+    <col min="2" max="2" width="16.140625" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" customWidth="1"/>
     <col min="4" max="4" width="13" customWidth="1"/>
-    <col min="5" max="5" width="15.5" customWidth="1"/>
-    <col min="6" max="6" width="10.1640625" customWidth="1"/>
-    <col min="7" max="7" width="9.6640625" customWidth="1"/>
+    <col min="5" max="5" width="15.42578125" customWidth="1"/>
+    <col min="6" max="6" width="10.140625" customWidth="1"/>
+    <col min="7" max="7" width="9.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>24</v>
       </c>
@@ -2095,7 +2099,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>40</v>
       </c>
@@ -2122,7 +2126,7 @@
         <v>0.50226155483333335</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>38</v>
       </c>
@@ -2149,7 +2153,7 @@
         <v>0.50071407800000001</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>41</v>
       </c>
@@ -2176,7 +2180,7 @@
         <v>0.47683879266666668</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>42</v>
       </c>
@@ -2203,7 +2207,7 @@
         <v>0.32228154999999997</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>43</v>
       </c>
@@ -2230,7 +2234,7 @@
         <v>0.3499723435</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>44</v>
       </c>
@@ -2257,7 +2261,7 @@
         <v>0.182635138</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>45</v>
       </c>
@@ -2284,7 +2288,7 @@
         <v>0.45364865333333332</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>46</v>
       </c>
@@ -2311,7 +2315,7 @@
         <v>0.20571497716666667</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>47</v>
       </c>
@@ -2338,7 +2342,7 @@
         <v>0.20571497716666667</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>31</v>
       </c>
@@ -2365,7 +2369,7 @@
         <v>0.55825067566666664</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>32</v>
       </c>
@@ -2392,7 +2396,7 @@
         <v>0.52787791566666664</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>48</v>
       </c>
@@ -2419,7 +2423,7 @@
         <v>0.50519873549999994</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>49</v>
       </c>
@@ -2446,7 +2450,7 @@
         <v>0.50226155483333335</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>30</v>
       </c>
@@ -2473,7 +2477,7 @@
         <v>0.31624555833333329</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>33</v>
       </c>
@@ -2500,7 +2504,7 @@
         <v>0.55055943233333327</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>34</v>
       </c>
@@ -2527,7 +2531,7 @@
         <v>0.5499720216666667</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>35</v>
       </c>
@@ -2554,7 +2558,7 @@
         <v>0.52090484549999994</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>36</v>
       </c>
@@ -2581,7 +2585,7 @@
         <v>0.54256848116666656</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>37</v>
       </c>
@@ -2608,7 +2612,7 @@
         <v>0.55330203150000001</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>50</v>
       </c>
@@ -2635,7 +2639,7 @@
         <v>0.54449444483333342</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>51</v>
       </c>
@@ -2672,20 +2676,20 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2027AD00-FE09-4B89-806B-EB77AB6D106B}">
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="11" customWidth="1"/>
-    <col min="3" max="3" width="13.1640625" customWidth="1"/>
-    <col min="4" max="4" width="12.5" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" customWidth="1"/>
+    <col min="4" max="4" width="12.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>24</v>
       </c>
@@ -2702,7 +2706,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>52</v>
       </c>
@@ -2720,7 +2724,7 @@
         <v>0.51611587133333325</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>53</v>
       </c>
@@ -2738,7 +2742,7 @@
         <v>0.50224398233333334</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>54</v>
       </c>
@@ -2756,7 +2760,7 @@
         <v>0.48429212566666663</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>55</v>
       </c>
@@ -2774,7 +2778,7 @@
         <v>0.47694818466666672</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>56</v>
       </c>
@@ -2792,7 +2796,7 @@
         <v>0.52713178266666672</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>57</v>
       </c>
@@ -2810,7 +2814,7 @@
         <v>0.48102815166666663</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>58</v>
       </c>
@@ -2828,7 +2832,7 @@
         <v>0.48143614833333331</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>59</v>
       </c>
@@ -2846,7 +2850,7 @@
         <v>0.51774785800000001</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>60</v>
       </c>
@@ -2864,7 +2868,7 @@
         <v>0.50061199533333334</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>61</v>
       </c>
@@ -2882,7 +2886,7 @@
         <v>0.44879640966666662</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>62</v>
       </c>
@@ -2900,7 +2904,7 @@
         <v>0.47735618099999999</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>63</v>
       </c>
@@ -2918,7 +2922,7 @@
         <v>0.47980416166666667</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>64</v>
       </c>
@@ -2936,128 +2940,146 @@
         <v>0.47246022033333329</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>73</v>
+      </c>
+      <c r="B15">
+        <v>0.41860465116279</v>
+      </c>
+      <c r="C15">
+        <v>0.43084455324357401</v>
+      </c>
+      <c r="D15">
+        <v>0.476132190942472</v>
+      </c>
+      <c r="E15" s="2">
+        <f>AVERAGE(Table3[[#This Row],[bleu_acc]:[bluert_acc]])</f>
+        <v>0.44186046511627869</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>65</v>
       </c>
-      <c r="B15">
+      <c r="B16">
         <v>0.47123622999999998</v>
       </c>
-      <c r="C15">
+      <c r="C16">
         <v>0.47368421100000002</v>
       </c>
-      <c r="D15">
+      <c r="D16">
         <v>0.52753978000000001</v>
       </c>
-      <c r="E15">
+      <c r="E16">
         <f>AVERAGE(Table3[[#This Row],[bleu_acc]:[bluert_acc]])</f>
         <v>0.49082007366666663</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>66</v>
       </c>
-      <c r="B16">
+      <c r="B17">
         <v>0.44675642599999998</v>
       </c>
-      <c r="C16">
+      <c r="C17">
         <v>0.457772338</v>
       </c>
-      <c r="D16">
+      <c r="D17">
         <v>0.51652386800000005</v>
       </c>
-      <c r="E16">
+      <c r="E17">
         <f>AVERAGE(Table3[[#This Row],[bleu_acc]:[bluert_acc]])</f>
         <v>0.47368421066666661</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>67</v>
       </c>
-      <c r="B17">
+      <c r="B18">
         <v>0.47368421100000002</v>
       </c>
-      <c r="C17">
+      <c r="C18">
         <v>0.487148103</v>
       </c>
-      <c r="D17">
+      <c r="D18">
         <v>0.54712362299999995</v>
       </c>
-      <c r="E17">
+      <c r="E18">
         <f>AVERAGE(Table3[[#This Row],[bleu_acc]:[bluert_acc]])</f>
         <v>0.50265197900000003</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>68</v>
       </c>
-      <c r="B18">
+      <c r="B19">
         <v>0.42717258299999999</v>
       </c>
-      <c r="C18">
+      <c r="C19">
         <v>0.44063647500000003</v>
       </c>
-      <c r="D18">
+      <c r="D19">
         <v>0.51040391699999998</v>
       </c>
-      <c r="E18">
+      <c r="E19">
         <f>AVERAGE(Table3[[#This Row],[bleu_acc]:[bluert_acc]])</f>
         <v>0.45940432499999995</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>69</v>
       </c>
-      <c r="B19">
+      <c r="B20">
         <v>0.42594859200000001</v>
       </c>
-      <c r="C19">
+      <c r="C20">
         <v>0.44675642599999998</v>
       </c>
-      <c r="D19">
+      <c r="D20">
         <v>0.50305997599999996</v>
       </c>
-      <c r="E19">
+      <c r="E20">
         <f>AVERAGE(Table3[[#This Row],[bleu_acc]:[bluert_acc]])</f>
         <v>0.45858833133333327</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>70</v>
       </c>
-      <c r="B20">
+      <c r="B21">
         <v>0.44553243599999998</v>
       </c>
-      <c r="C20">
+      <c r="C21">
         <v>0.45899632800000001</v>
       </c>
-      <c r="D20">
+      <c r="D21">
         <v>0.50428396600000003</v>
       </c>
-      <c r="E20">
+      <c r="E21">
         <f>AVERAGE(Table3[[#This Row],[bleu_acc]:[bluert_acc]])</f>
         <v>0.46960424333333334</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>71</v>
       </c>
-      <c r="B21">
+      <c r="B22">
         <v>0.40881272899999999</v>
       </c>
-      <c r="C21">
+      <c r="C22">
         <v>0.428396573</v>
       </c>
-      <c r="D21">
+      <c r="D22">
         <v>0.454100367</v>
       </c>
-      <c r="E21">
+      <c r="E22">
         <f>AVERAGE(Table3[[#This Row],[bleu_acc]:[bluert_acc]])</f>
         <v>0.43043655633333328</v>
       </c>

</xml_diff>

<commit_message>
minor changes and rename
</commit_message>
<xml_diff>
--- a/Final Evaluation/merged_averages.xlsx
+++ b/Final Evaluation/merged_averages.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pink\Documents\Study\Intelligent Systems\COS30018-Mitigate-Hallucination\Final Evaluation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://liveswinburneeduau-my.sharepoint.com/personal/104220556_student_swin_edu_au/Documents/Swinburne/Intelligent Systems/Hallucination-Mitigation/Final Evaluation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F25F110-C830-44FC-B0D1-76855E80830F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="47" documentId="13_ncr:1_{9F25F110-C830-44FC-B0D1-76855E80830F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3317CA75-6A79-4399-A005-6F53EA0A7A8C}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21840" tabRatio="549" activeTab="3" xr2:uid="{6A54DB1A-C799-4116-88B3-55941F091460}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="549" activeTab="3" xr2:uid="{6A54DB1A-C799-4116-88B3-55941F091460}"/>
   </bookViews>
   <sheets>
     <sheet name="Med-Halt" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="73">
   <si>
     <t>FAKE Accuracy_pred</t>
   </si>
@@ -241,46 +241,28 @@
     <t>bleurt_acc</t>
   </si>
   <si>
-    <t>History_2</t>
-  </si>
-  <si>
-    <t>History_3</t>
-  </si>
-  <si>
-    <t>History_3_old</t>
-  </si>
-  <si>
-    <t>History_4</t>
-  </si>
-  <si>
-    <t>Hisory</t>
-  </si>
-  <si>
-    <t>New_2</t>
-  </si>
-  <si>
-    <t>New_3</t>
-  </si>
-  <si>
-    <t>New_4</t>
-  </si>
-  <si>
-    <t>New_4_old</t>
-  </si>
-  <si>
-    <t>New_5</t>
-  </si>
-  <si>
-    <t>New</t>
-  </si>
-  <si>
-    <t>Original</t>
+    <t>version</t>
+  </si>
+  <si>
+    <t>H1</t>
+  </si>
+  <si>
+    <t>H2</t>
+  </si>
+  <si>
+    <t>H3</t>
+  </si>
+  <si>
+    <t>H4</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="166" formatCode="0.0000"/>
+  </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -758,10 +740,14 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="12"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -807,9 +793,21 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="9">
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <numFmt numFmtId="166" formatCode="0.0000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="0.0000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="0.0000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="0.0000"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -859,7 +857,7 @@
     <tableColumn id="17" xr3:uid="{1125E03B-3007-4C50-ADC2-4068DA339121}" name="NOTA meteor_score"/>
     <tableColumn id="18" xr3:uid="{950668D7-80FC-4AA6-BD23-AABC242C15B3}" name="NOTA rouge_1"/>
     <tableColumn id="19" xr3:uid="{7C8752D9-DDB5-4736-90A3-07B2A6D9772F}" name="NOTA rouge_l"/>
-    <tableColumn id="20" xr3:uid="{61D1E807-C74A-4DD6-8D8E-19294302F4EB}" name="Average" dataDxfId="4">
+    <tableColumn id="20" xr3:uid="{61D1E807-C74A-4DD6-8D8E-19294302F4EB}" name="Average" dataDxfId="8">
       <calculatedColumnFormula>AVERAGE(Table1[[#This Row],[FAKE Accuracy_pred]:[NOTA rouge_l]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -874,11 +872,11 @@
     <tableColumn id="1" xr3:uid="{B5197018-447D-40E9-8DA3-30DD43EAEC05}" name="model"/>
     <tableColumn id="2" xr3:uid="{79783DF6-B10D-4B1D-ADBB-1F916059C49D}" name="Accuracy_pred"/>
     <tableColumn id="3" xr3:uid="{144A4880-C521-41D5-B355-0EC9727D3E13}" name="Accuracy_ref"/>
-    <tableColumn id="4" xr3:uid="{62CA84C3-3DE7-41E3-91D6-92AEC38F1FFB}" name="bleu_score" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{62CA84C3-3DE7-41E3-91D6-92AEC38F1FFB}" name="bleu_score" dataDxfId="7"/>
     <tableColumn id="5" xr3:uid="{28D4F70E-F5A7-4CBC-B9EC-92FA3CADE083}" name="meteor_score"/>
     <tableColumn id="6" xr3:uid="{27DC8526-E241-4CD9-B1A0-64B29FBF3E26}" name="rouge_1"/>
     <tableColumn id="7" xr3:uid="{25A451DE-B218-4ED2-9535-EAF5FFC013EC}" name="rouge_l"/>
-    <tableColumn id="8" xr3:uid="{B7D0D997-5BDB-4439-B55F-A46B61F80F3E}" name="Average" dataDxfId="2">
+    <tableColumn id="8" xr3:uid="{B7D0D997-5BDB-4439-B55F-A46B61F80F3E}" name="Average" dataDxfId="6">
       <calculatedColumnFormula>AVERAGE(Table2[[#This Row],[Accuracy_pred]:[rouge_l]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -894,7 +892,7 @@
     <tableColumn id="2" xr3:uid="{43A76758-9B3A-4B48-B95E-240B62A5A2C2}" name="bleu_acc"/>
     <tableColumn id="3" xr3:uid="{FE50AF38-6D21-4CA3-A7D1-F4F34A493C04}" name="rouge1_acc"/>
     <tableColumn id="4" xr3:uid="{11D72553-292B-4A27-A6A4-242EA9BD3090}" name="bluert_acc"/>
-    <tableColumn id="5" xr3:uid="{B101CC56-035B-4C29-AC38-A417FA380D11}" name="Average" dataDxfId="1">
+    <tableColumn id="5" xr3:uid="{B101CC56-035B-4C29-AC38-A417FA380D11}" name="Average" dataDxfId="5">
       <calculatedColumnFormula>AVERAGE(Table3[[#This Row],[bleu_acc]:[bluert_acc]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -903,13 +901,13 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{3E0B2FA9-B02D-4545-A84C-ADBB16EA8719}" name="Table4" displayName="Table4" ref="A1:E13" totalsRowShown="0">
-  <autoFilter ref="A1:E13" xr:uid="{3E0B2FA9-B02D-4545-A84C-ADBB16EA8719}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{3E0B2FA9-B02D-4545-A84C-ADBB16EA8719}" name="Table4" displayName="Table4" ref="A1:E11" totalsRowShown="0">
+  <autoFilter ref="A1:E11" xr:uid="{3E0B2FA9-B02D-4545-A84C-ADBB16EA8719}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{B6691E61-075A-47D1-B9B2-7BAD670FE3C2}" name="model"/>
-    <tableColumn id="2" xr3:uid="{DC1D90E4-7A9E-4490-97DC-98806F04F5B3}" name="bleu_acc"/>
-    <tableColumn id="3" xr3:uid="{92754137-65B2-4698-93C7-E3D12E15885E}" name="rouge1_acc"/>
-    <tableColumn id="4" xr3:uid="{1AC4AFA7-7EC3-421B-8143-A93F11C40ABD}" name="bleurt_acc"/>
+    <tableColumn id="1" xr3:uid="{B6691E61-075A-47D1-B9B2-7BAD670FE3C2}" name="version" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{DC1D90E4-7A9E-4490-97DC-98806F04F5B3}" name="bleu_acc" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{92754137-65B2-4698-93C7-E3D12E15885E}" name="rouge1_acc" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{1AC4AFA7-7EC3-421B-8143-A93F11C40ABD}" name="bleurt_acc" dataDxfId="1"/>
     <tableColumn id="5" xr3:uid="{E0813EA2-EF6D-4EBB-8FCC-A2B7092A974A}" name="Average" dataDxfId="0">
       <calculatedColumnFormula>AVERAGE(Table4[[#This Row],[bleu_acc]:[bleurt_acc]])</calculatedColumnFormula>
     </tableColumn>
@@ -2947,24 +2945,24 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E1D436B-0772-4F28-A226-6511B12E8139}">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11" customWidth="1"/>
-    <col min="3" max="3" width="13.140625" customWidth="1"/>
-    <col min="4" max="4" width="12.42578125" customWidth="1"/>
+    <col min="1" max="1" width="7" customWidth="1"/>
+    <col min="2" max="2" width="9.7109375" customWidth="1"/>
+    <col min="3" max="3" width="11.140625" customWidth="1"/>
+    <col min="4" max="4" width="10.42578125" customWidth="1"/>
     <col min="5" max="6" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>24</v>
+        <v>68</v>
       </c>
       <c r="B1" t="s">
         <v>25</v>
@@ -2980,219 +2978,183 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>68</v>
-      </c>
-      <c r="B2">
+      <c r="A2" s="3">
+        <v>0</v>
+      </c>
+      <c r="B2" s="4">
+        <v>0.43574051407588699</v>
+      </c>
+      <c r="C2" s="4">
+        <v>0.438188494492044</v>
+      </c>
+      <c r="D2" s="4">
+        <v>0.58506731946144397</v>
+      </c>
+      <c r="E2" s="4">
+        <f>AVERAGE(Table4[[#This Row],[bleu_acc]:[bleurt_acc]])</f>
+        <v>0.48633210934312499</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="3">
+        <v>1</v>
+      </c>
+      <c r="B3" s="4">
+        <v>0.38800489596083199</v>
+      </c>
+      <c r="C3" s="4">
+        <v>0.428396572827417</v>
+      </c>
+      <c r="D3" s="4">
+        <v>0.48714810281517701</v>
+      </c>
+      <c r="E3" s="4">
+        <f>AVERAGE(Table4[[#This Row],[bleu_acc]:[bleurt_acc]])</f>
+        <v>0.43451652386780865</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
+        <v>2</v>
+      </c>
+      <c r="B4" s="4">
+        <v>0.446756425948592</v>
+      </c>
+      <c r="C4" s="4">
+        <v>0.46878824969400201</v>
+      </c>
+      <c r="D4" s="4">
+        <v>0.53121175030599699</v>
+      </c>
+      <c r="E4" s="4">
+        <f>AVERAGE(Table4[[#This Row],[bleu_acc]:[bleurt_acc]])</f>
+        <v>0.48225214198286365</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="3">
+        <v>3</v>
+      </c>
+      <c r="B5" s="4">
+        <v>0.50795593635250902</v>
+      </c>
+      <c r="C5" s="4">
+        <v>0.53488372093023195</v>
+      </c>
+      <c r="D5" s="4">
+        <v>0.61689106487148104</v>
+      </c>
+      <c r="E5" s="4">
+        <f>AVERAGE(Table4[[#This Row],[bleu_acc]:[bleurt_acc]])</f>
+        <v>0.55324357405140734</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="3">
+        <v>4</v>
+      </c>
+      <c r="B6" s="4">
+        <v>0.494492044063647</v>
+      </c>
+      <c r="C6" s="4">
+        <v>0.52509179926560501</v>
+      </c>
+      <c r="D6" s="4">
+        <v>0.581395348837209</v>
+      </c>
+      <c r="E6" s="4">
+        <f>AVERAGE(Table4[[#This Row],[bleu_acc]:[bleurt_acc]])</f>
+        <v>0.53365973072215367</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="3">
+        <v>5</v>
+      </c>
+      <c r="B7" s="4">
+        <v>0.438188494492044</v>
+      </c>
+      <c r="C7" s="4">
+        <v>0.45042839657282702</v>
+      </c>
+      <c r="D7" s="4">
+        <v>0.52509179926560501</v>
+      </c>
+      <c r="E7" s="4">
+        <f>AVERAGE(Table4[[#This Row],[bleu_acc]:[bleurt_acc]])</f>
+        <v>0.47123623011015869</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B8" s="4">
+        <v>0.26805385556915501</v>
+      </c>
+      <c r="C8" s="4">
+        <v>0.42105263157894701</v>
+      </c>
+      <c r="D8" s="4">
+        <v>0.52753977968176202</v>
+      </c>
+      <c r="E8" s="4">
+        <f>AVERAGE(Table4[[#This Row],[bleu_acc]:[bleurt_acc]])</f>
+        <v>0.40554875560995468</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B9" s="4">
         <v>0.69889840881272902</v>
       </c>
-      <c r="C2">
+      <c r="C9" s="4">
         <v>0.75764993880048903</v>
       </c>
-      <c r="D2">
+      <c r="D9" s="4">
         <v>0.77600979192166397</v>
       </c>
-      <c r="E2">
+      <c r="E9" s="4">
         <f>AVERAGE(Table4[[#This Row],[bleu_acc]:[bleurt_acc]])</f>
         <v>0.74418604651162734</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>69</v>
-      </c>
-      <c r="B3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B10" s="4">
         <v>0.70379436964504205</v>
       </c>
-      <c r="C3">
+      <c r="C10" s="4">
         <v>0.77233782129742901</v>
       </c>
-      <c r="D3">
+      <c r="D10" s="4">
         <v>0.78212974296205595</v>
       </c>
-      <c r="E3">
+      <c r="E10" s="4">
         <f>AVERAGE(Table4[[#This Row],[bleu_acc]:[bleurt_acc]])</f>
         <v>0.75275397796817567</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>70</v>
-      </c>
-      <c r="B4">
-        <v>0.70379436964504205</v>
-      </c>
-      <c r="C4">
-        <v>0.77233782129742901</v>
-      </c>
-      <c r="D4">
-        <v>0.78212974296205595</v>
-      </c>
-      <c r="E4">
-        <f>AVERAGE(Table4[[#This Row],[bleu_acc]:[bleurt_acc]])</f>
-        <v>0.75275397796817567</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>71</v>
-      </c>
-      <c r="B5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B11" s="4">
         <v>0.61933904528763695</v>
       </c>
-      <c r="C5">
+      <c r="C11" s="4">
         <v>0.70991432068543403</v>
       </c>
-      <c r="D5">
+      <c r="D11" s="4">
         <v>0.73929008567931398</v>
       </c>
-      <c r="E5">
+      <c r="E11" s="4">
         <f>AVERAGE(Table4[[#This Row],[bleu_acc]:[bleurt_acc]])</f>
         <v>0.68951448388412828</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>72</v>
-      </c>
-      <c r="B6">
-        <v>0.26805385556915501</v>
-      </c>
-      <c r="C6">
-        <v>0.42105263157894701</v>
-      </c>
-      <c r="D6">
-        <v>0.52753977968176202</v>
-      </c>
-      <c r="E6">
-        <f>AVERAGE(Table4[[#This Row],[bleu_acc]:[bleurt_acc]])</f>
-        <v>0.40554875560995468</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>73</v>
-      </c>
-      <c r="B7">
-        <v>0.446756425948592</v>
-      </c>
-      <c r="C7">
-        <v>0.46878824969400201</v>
-      </c>
-      <c r="D7">
-        <v>0.53121175030599699</v>
-      </c>
-      <c r="E7">
-        <f>AVERAGE(Table4[[#This Row],[bleu_acc]:[bleurt_acc]])</f>
-        <v>0.48225214198286365</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>74</v>
-      </c>
-      <c r="B8">
-        <v>0.50795593635250902</v>
-      </c>
-      <c r="C8">
-        <v>0.53488372093023195</v>
-      </c>
-      <c r="D8">
-        <v>0.61689106487148104</v>
-      </c>
-      <c r="E8">
-        <f>AVERAGE(Table4[[#This Row],[bleu_acc]:[bleurt_acc]])</f>
-        <v>0.55324357405140734</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>75</v>
-      </c>
-      <c r="B9">
-        <v>0.494492044063647</v>
-      </c>
-      <c r="C9">
-        <v>0.52509179926560501</v>
-      </c>
-      <c r="D9">
-        <v>0.581395348837209</v>
-      </c>
-      <c r="E9">
-        <f>AVERAGE(Table4[[#This Row],[bleu_acc]:[bleurt_acc]])</f>
-        <v>0.53365973072215367</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>76</v>
-      </c>
-      <c r="B10">
-        <v>0.53121175030599699</v>
-      </c>
-      <c r="C10">
-        <v>0.55446756425948596</v>
-      </c>
-      <c r="D10">
-        <v>0.59730722154222704</v>
-      </c>
-      <c r="E10">
-        <f>AVERAGE(Table4[[#This Row],[bleu_acc]:[bleurt_acc]])</f>
-        <v>0.56099551203590325</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>77</v>
-      </c>
-      <c r="B11">
-        <v>0.438188494492044</v>
-      </c>
-      <c r="C11">
-        <v>0.45042839657282702</v>
-      </c>
-      <c r="D11">
-        <v>0.52509179926560501</v>
-      </c>
-      <c r="E11">
-        <f>AVERAGE(Table4[[#This Row],[bleu_acc]:[bleurt_acc]])</f>
-        <v>0.47123623011015869</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>78</v>
-      </c>
-      <c r="B12">
-        <v>0.38800489596083199</v>
-      </c>
-      <c r="C12">
-        <v>0.428396572827417</v>
-      </c>
-      <c r="D12">
-        <v>0.48714810281517701</v>
-      </c>
-      <c r="E12">
-        <f>AVERAGE(Table4[[#This Row],[bleu_acc]:[bleurt_acc]])</f>
-        <v>0.43451652386780865</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>79</v>
-      </c>
-      <c r="B13">
-        <v>0.43574051407588699</v>
-      </c>
-      <c r="C13">
-        <v>0.438188494492044</v>
-      </c>
-      <c r="D13">
-        <v>0.58506731946144397</v>
-      </c>
-      <c r="E13">
-        <f>AVERAGE(Table4[[#This Row],[bleu_acc]:[bleurt_acc]])</f>
-        <v>0.48633210934312499</v>
       </c>
     </row>
   </sheetData>

</xml_diff>